<commit_message>
"Script funcional, atriibuição de triangulos / cirulos no nesting"
</commit_message>
<xml_diff>
--- a/Versao-FInal/codigo_database.xlsx
+++ b/Versao-FInal/codigo_database.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B6"/>
@@ -874,6 +874,176 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>VDS1832</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15/10/2025 07:28:26</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>VDS1833</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>15/10/2025 07:48:59</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1922</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>VDS1834</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:09:49</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Chorão-as-rosas</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>VDS1835</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:11:46</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Noroaco</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>VDS1836</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:15:13</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Noroaco</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>VDS1837</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:19:27</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>VDS1838</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:19:39</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>VDS1839</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:19:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>VDS1840</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:42:19</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>VDS1841</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15/10/2025 10:42:43</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
'Att - Antes do almoco"
</commit_message>
<xml_diff>
--- a/Versao-FInal/codigo_database.xlsx
+++ b/Versao-FInal/codigo_database.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B6"/>
@@ -1044,6 +1044,159 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>VDS1842</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:01:13</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1585</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>VDS1843</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:05:59</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>555555555</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>VDS1844</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:06:15</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>555555555</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>VDS1845</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:06:34</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>555555555</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>VDS1846</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:06:56</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>555555555</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>VDS1847</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:08:04</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>555555555</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>VDS1848</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:08:32</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>555555555</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>VDS1849</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:34:44</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>123563</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>VDS1850</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>15/10/2025 11:34:50</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>123563</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>